<commit_message>
Update Tandy TRS-80 Color Computer 2 Bill of Materials - 8857625 & 8857636.xlsx
</commit_message>
<xml_diff>
--- a/Tandy/TRS-80/Tandy TRS-80 Color Computer 2/Documents/Tandy TRS-80 Color Computer 2 Bill of Materials - 8857625 & 8857636.xlsx
+++ b/Tandy/TRS-80/Tandy TRS-80 Color Computer 2/Documents/Tandy TRS-80 Color Computer 2 Bill of Materials - 8857625 & 8857636.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Retro-Schematics\Tandy\TRS-80\Tandy TRS-80 Color Computer 2\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CE0D3A-2F26-4711-A006-FC52D261EC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9D48A9-260A-4BA5-9E1B-C47D568B6C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="220">
   <si>
     <t>ITEM</t>
   </si>
@@ -689,6 +689,9 @@
   </si>
   <si>
     <t>MC6809E, CPU</t>
+  </si>
+  <si>
+    <t>* USED ON 8857636 EXTENDED BASIC PCB ONLY</t>
   </si>
 </sst>
 </file>
@@ -2795,10 +2798,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5A9B8B8-E328-4ED1-B76D-4850401F3FF1}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3083,6 +3086,11 @@
         <v>8409008</v>
       </c>
     </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>219</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>